<commit_message>
i kinda change a liitle bit everything but it worth it the project is done
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Data after SMOTE-ENC" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="DATA after K-Fold" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SHAP_Sensitivity" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -109,13 +110,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -3972,52 +3979,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Age</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Gender</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Blood Oxygen Level (%)</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Body Temperature (°C)</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Heart Rate (bpm)</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Physical Activity Level (METs)</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Overall Health Score</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>Sleep Duration (hours)</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Hydration Level (liters)</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">Stress Level </t>
         </is>
@@ -8523,52 +8530,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Age</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Gender</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Blood Oxygen Level (%)</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Body Temperature (°C)</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Heart Rate (bpm)</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Physical Activity Level (METs)</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Overall Health Score</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>Sleep Duration (hours)</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Hydration Level (liters)</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">Stress Level </t>
         </is>
@@ -13052,6 +13059,127 @@
       </c>
       <c r="J141" t="n">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Sensitivity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Overall Health Score</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1.130897959183673</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Blood Oxygen Level (%)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5701801303854873</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.4904221938775498</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.4200868764172339</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Physical Activity Level (METs)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.398206065759637</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Heart Rate (bpm)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.3439384920634915</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Hydration Level (liters)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.314635629251701</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sleep Duration (hours)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.2685301870748297</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Body Temperature (°C)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.2500364229024942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>